<commit_message>
data added 2015-2023 and table 1 organized
</commit_message>
<xml_diff>
--- a/data/state_to_state_migration/2023.xlsx
+++ b/data/state_to_state_migration/2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nycdoitt-my.sharepoint.com/personal/lcatalan_nycopportunity_nyc_gov/Documents/Documents/dev/migration-flows/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nycdoitt-my.sharepoint.com/personal/lcatalan_nycopportunity_nyc_gov/Documents/Documents/dev/migration-flows/data/state_to_state_migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{EF66FCB7-F138-4FF2-A76D-E27024EFACDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE17CFE0-A07D-450E-8077-A9371792CFEE}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{EF66FCB7-F138-4FF2-A76D-E27024EFACDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CECD0633-D05C-470F-B752-62049A5B9680}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26760" yWindow="1635" windowWidth="25005" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -1612,6 +1612,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -1901,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DQ74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2266,7 +2270,7 @@
       <c r="DH3" s="2"/>
       <c r="DI3" s="2"/>
     </row>
-    <row r="4" spans="1:119" s="10" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:119" s="10" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -23380,8 +23384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E483CEC1-CE88-49F2-BE11-8FE05131BA45}">
   <dimension ref="A1:N84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>